<commit_message>
Updated the entities sheet for additional info
</commit_message>
<xml_diff>
--- a/infodev/99-exceldmd/Base Data Model_RW.xlsx
+++ b/infodev/99-exceldmd/Base Data Model_RW.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nagamba\Desktop\RiverWorks DMD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git-ui\dataplatform-sampledata\dataplatform-sampledata\infodev\99-exceldmd\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="HELP" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
     <definedName name="_Attribute_Name">'[1]S7 - Attribute'!$E$2:$E$1048576</definedName>
     <definedName name="_Boolean">'[1]20170320 065838_DataModel_Templ'!#REF!</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">ATTRIBUTES!$A$1:$AE$67</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'E-A-R-C MODEL'!$A$1:$AA$9</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'E-A-R-C MODEL'!$A$1:$AA$161</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">ENTITIES!$A$1:$D$1</definedName>
     <definedName name="_RefDataAttribute">ATTRIBUTES!#REF!</definedName>
     <definedName name="RefDataAttribute">ATTRIBUTES!#REF!</definedName>
@@ -171,7 +171,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="704" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="838" uniqueCount="271">
   <si>
     <t>ACTION</t>
   </si>
@@ -257,9 +257,6 @@
     <t>DEFAULT VALUE</t>
   </si>
   <si>
-    <t>SKU</t>
-  </si>
-  <si>
     <t>sku</t>
   </si>
   <si>
@@ -915,6 +912,78 @@
   </si>
   <si>
     <t>Last Modified Date and Time</t>
+  </si>
+  <si>
+    <t>style</t>
+  </si>
+  <si>
+    <t>vendor</t>
+  </si>
+  <si>
+    <t>Style</t>
+  </si>
+  <si>
+    <t>Sku</t>
+  </si>
+  <si>
+    <t>Vendor</t>
+  </si>
+  <si>
+    <t>Product Sku</t>
+  </si>
+  <si>
+    <t>mdm Id</t>
+  </si>
+  <si>
+    <t>model Number</t>
+  </si>
+  <si>
+    <t>available Date</t>
+  </si>
+  <si>
+    <t>last Modified Datetime</t>
+  </si>
+  <si>
+    <t>repository Link</t>
+  </si>
+  <si>
+    <t>storage Image</t>
+  </si>
+  <si>
+    <t>demo Video</t>
+  </si>
+  <si>
+    <t>datasheet Link</t>
+  </si>
+  <si>
+    <t>warranty Included</t>
+  </si>
+  <si>
+    <t>service Contract Duration</t>
+  </si>
+  <si>
+    <t>apply VAT</t>
+  </si>
+  <si>
+    <t>case Info</t>
+  </si>
+  <si>
+    <t>vendor Name</t>
+  </si>
+  <si>
+    <t>buyer Name</t>
+  </si>
+  <si>
+    <t>web Discount</t>
+  </si>
+  <si>
+    <t>web Price</t>
+  </si>
+  <si>
+    <t>sku color</t>
+  </si>
+  <si>
+    <t>category</t>
   </si>
 </sst>
 </file>
@@ -1606,7 +1675,7 @@
         <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1614,7 +1683,7 @@
         <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1622,39 +1691,39 @@
         <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -1692,13 +1761,13 @@
   <sheetData>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B4" s="11" t="s">
         <v>22</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E4" s="12" t="s">
         <v>4</v>
@@ -1709,10 +1778,10 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D5" s="11">
         <v>1</v>
@@ -1721,15 +1790,15 @@
         <v>7</v>
       </c>
       <c r="F5" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D6" s="11">
         <v>2</v>
@@ -1738,15 +1807,15 @@
         <v>8</v>
       </c>
       <c r="F6" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D7" s="11">
         <v>3</v>
@@ -1755,29 +1824,29 @@
         <v>9</v>
       </c>
       <c r="F7" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D8" s="11">
         <v>4</v>
       </c>
       <c r="E8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F8" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="16" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B9" s="17" t="s">
         <v>21</v>
@@ -1786,10 +1855,10 @@
         <v>5</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F9" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -1801,10 +1870,10 @@
         <v>6</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F10" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -1816,10 +1885,10 @@
         <v>7</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F11" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -1831,7 +1900,7 @@
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="22"/>
       <c r="B13" s="23" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -1853,11 +1922,11 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="G16" sqref="G16"/>
+      <selection pane="bottomLeft" activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1879,34 +1948,68 @@
         <v>2</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
+      <c r="B2" s="30" t="s">
+        <v>247</v>
+      </c>
+      <c r="C2" s="30" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B3" s="30" t="s">
+        <v>121</v>
+      </c>
+      <c r="C3" s="30" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B4" s="30" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="30" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B5" s="30" t="s">
+        <v>248</v>
+      </c>
+      <c r="C5" s="30" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B6" s="30" t="s">
+        <v>186</v>
+      </c>
+      <c r="C6" s="30" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B7" s="30" t="s">
+        <v>117</v>
+      </c>
+      <c r="C7" s="30" t="s">
         <v>118</v>
       </c>
-      <c r="C2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>187</v>
-      </c>
-      <c r="C3" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.25"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B8" s="30" t="s">
+        <v>199</v>
+      </c>
+      <c r="C8" s="30" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C9" s="30"/>
+    </row>
   </sheetData>
   <customSheetViews>
     <customSheetView guid="{BF8E1B46-AD75-6E4F-85B7-6E6C75F2AAA2}" scale="150">
@@ -1929,11 +2032,11 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:AF67"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="80" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="80" workbookViewId="0">
+      <pane xSplit="4" ySplit="1" topLeftCell="F41" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H17" sqref="H17"/>
+      <selection pane="bottomRight" activeCell="B61" sqref="B61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1981,10 +2084,10 @@
         <v>3</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F1" s="6" t="s">
         <v>2</v>
@@ -1993,19 +2096,19 @@
         <v>20</v>
       </c>
       <c r="H1" s="25" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J1" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="K1" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>110</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>111</v>
       </c>
       <c r="M1" s="4" t="s">
         <v>10</v>
@@ -2038,51 +2141,51 @@
         <v>19</v>
       </c>
       <c r="W1" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="X1" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="X1" s="6" t="s">
+      <c r="Y1" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="Y1" s="6" t="s">
+      <c r="Z1" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="Z1" s="6" t="s">
+      <c r="AA1" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="AA1" s="6" t="s">
+      <c r="AB1" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="AB1" s="6" t="s">
-        <v>86</v>
-      </c>
       <c r="AC1" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="AD1" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="AE1" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="AD1" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="AE1" s="6" t="s">
-        <v>102</v>
-      </c>
       <c r="AF1" s="6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="2" spans="1:32" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="27" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C2" s="27" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E2" s="27" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F2" s="27" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G2" s="27" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H2" s="29"/>
       <c r="M2" s="31"/>
@@ -2098,19 +2201,19 @@
     </row>
     <row r="3" spans="1:32" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B3" s="27" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C3" s="31" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E3" s="27" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F3" s="27" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G3" s="31" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H3" s="29"/>
       <c r="M3" s="31">
@@ -2130,19 +2233,19 @@
     </row>
     <row r="4" spans="1:32" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B4" s="27" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C4" s="31" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E4" s="27" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F4" s="27" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G4" s="31" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H4" s="29"/>
       <c r="M4" s="31"/>
@@ -2158,19 +2261,19 @@
     </row>
     <row r="5" spans="1:32" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B5" s="27" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C5" s="27" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E5" s="27" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F5" s="27" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G5" s="31" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H5" s="29"/>
       <c r="M5" s="31"/>
@@ -2186,19 +2289,19 @@
     </row>
     <row r="6" spans="1:32" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="27" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C6" s="27" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E6" s="27" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F6" s="27" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G6" s="27" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H6" s="29"/>
       <c r="M6" s="31"/>
@@ -2214,19 +2317,19 @@
     </row>
     <row r="7" spans="1:32" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B7" s="27" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C7" s="27" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E7" s="27" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F7" s="27" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G7" s="27" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H7" s="29"/>
       <c r="M7" s="31"/>
@@ -2242,56 +2345,56 @@
     </row>
     <row r="8" spans="1:32" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B8" s="27" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C8" s="27" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E8" s="27" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F8" s="27" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G8" s="27" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H8" s="29"/>
       <c r="S8" s="32"/>
     </row>
     <row r="9" spans="1:32" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B9" s="27" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C9" s="27" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E9" s="27" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F9" s="27" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="G9" s="27" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H9" s="29"/>
     </row>
     <row r="10" spans="1:32" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B10" s="27" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C10" s="27" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E10" s="27" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F10" s="27" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G10" s="27" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H10" s="29"/>
       <c r="M10" s="31"/>
@@ -2307,19 +2410,19 @@
     </row>
     <row r="11" spans="1:32" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B11" s="31" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C11" s="27" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E11" s="27" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F11" s="31" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G11" s="27" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H11" s="29"/>
       <c r="M11" s="31"/>
@@ -2335,19 +2438,19 @@
     </row>
     <row r="12" spans="1:32" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B12" s="27" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C12" s="27" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E12" s="27" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F12" s="27" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G12" s="27" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H12" s="29"/>
       <c r="M12" s="31"/>
@@ -2363,19 +2466,19 @@
     </row>
     <row r="13" spans="1:32" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B13" s="31" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C13" s="27" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E13" s="27" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F13" s="31" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G13" s="27" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H13" s="29"/>
       <c r="M13" s="31"/>
@@ -2391,19 +2494,19 @@
     </row>
     <row r="14" spans="1:32" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B14" s="27" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C14" s="27" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E14" s="27" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F14" s="27" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="G14" s="27" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="H14" s="29"/>
       <c r="O14" s="31"/>
@@ -2414,30 +2517,30 @@
         <v>2</v>
       </c>
       <c r="T14" s="27" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="U14" s="31" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="V14" s="31" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="15" spans="1:32" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B15" s="27" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C15" s="27" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E15" s="27" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F15" s="27" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G15" s="27" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="H15" s="29"/>
       <c r="P15" s="27">
@@ -2449,19 +2552,19 @@
     </row>
     <row r="16" spans="1:32" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B16" s="27" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C16" s="27" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E16" s="27" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F16" s="27" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G16" s="27" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="H16" s="29"/>
       <c r="P16" s="27">
@@ -2473,19 +2576,19 @@
     </row>
     <row r="17" spans="2:22" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B17" s="27" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C17" s="27" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E17" s="27" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F17" s="27" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G17" s="30" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H17" s="29"/>
       <c r="S17" s="27">
@@ -2494,154 +2597,154 @@
     </row>
     <row r="18" spans="2:22" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B18" s="27" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C18" s="27" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E18" s="27" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F18" s="27" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G18" s="27" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H18" s="29"/>
     </row>
     <row r="19" spans="2:22" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B19" s="27" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C19" s="31" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E19" s="27" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F19" s="27" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G19" s="31" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H19" s="29"/>
     </row>
     <row r="20" spans="2:22" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B20" s="27" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C20" s="31" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E20" s="27" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F20" s="27" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G20" s="31" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H20" s="29"/>
     </row>
     <row r="21" spans="2:22" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B21" s="27" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C21" s="31" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E21" s="27" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F21" s="27" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G21" s="31" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H21" s="29"/>
     </row>
     <row r="22" spans="2:22" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B22" s="27" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C22" s="31" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E22" s="27" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F22" s="27" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G22" s="31" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H22" s="29"/>
     </row>
     <row r="23" spans="2:22" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B23" s="27" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C23" s="27" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E23" s="27" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F23" s="27" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G23" s="27" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="H23" s="29"/>
     </row>
     <row r="24" spans="2:22" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B24" s="27" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C24" s="27" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E24" s="27" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F24" s="27" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G24" s="30" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H24" s="29"/>
       <c r="T24" s="27" t="s">
+        <v>177</v>
+      </c>
+      <c r="U24" s="27" t="s">
         <v>178</v>
       </c>
-      <c r="U24" s="27" t="s">
-        <v>179</v>
-      </c>
       <c r="V24" s="27" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="25" spans="2:22" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B25" s="27" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C25" s="31" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E25" s="31" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F25" s="31" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G25" s="31" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="H25" s="29"/>
       <c r="M25" s="31"/>
@@ -2657,19 +2760,19 @@
     </row>
     <row r="26" spans="2:22" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B26" s="31" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C26" s="31" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E26" s="31" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F26" s="31" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G26" s="31" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="H26" s="29"/>
       <c r="M26" s="31"/>
@@ -2689,19 +2792,19 @@
     </row>
     <row r="27" spans="2:22" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B27" s="31" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C27" s="31" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E27" s="31" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F27" s="31" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G27" s="31" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="H27" s="29"/>
       <c r="M27" s="31"/>
@@ -2719,19 +2822,19 @@
     </row>
     <row r="28" spans="2:22" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B28" s="31" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C28" s="31" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E28" s="31" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F28" s="31" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G28" s="31" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="H28" s="29"/>
       <c r="M28" s="31"/>
@@ -2749,19 +2852,19 @@
     </row>
     <row r="29" spans="2:22" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B29" s="31" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C29" s="31" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E29" s="31" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F29" s="31" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G29" s="31" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="H29" s="29"/>
       <c r="M29" s="31"/>
@@ -2779,19 +2882,19 @@
     </row>
     <row r="30" spans="2:22" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B30" s="31" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C30" s="31" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E30" s="31" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F30" s="27" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G30" s="31" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="H30" s="29"/>
       <c r="M30" s="31"/>
@@ -2809,19 +2912,19 @@
     </row>
     <row r="31" spans="2:22" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B31" s="31" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C31" s="31" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E31" s="31" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F31" s="31" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G31" s="31" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="H31" s="29"/>
       <c r="M31" s="31"/>
@@ -2839,253 +2942,253 @@
     </row>
     <row r="32" spans="2:22" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B32" s="27" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C32" s="27" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E32" s="27" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F32" s="27" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G32" s="27" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H32" s="29"/>
     </row>
     <row r="33" spans="2:22" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B33" s="27" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C33" s="27" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E33" s="27" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F33" s="27" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="G33" s="27" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H33" s="29"/>
     </row>
     <row r="34" spans="2:22" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B34" s="27" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C34" s="27" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E34" s="27" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F34" s="27" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G34" s="30" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H34" s="29"/>
     </row>
     <row r="35" spans="2:22" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B35" s="27" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C35" s="27" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E35" s="27" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F35" s="27" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="G35" s="27" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H35" s="29"/>
     </row>
     <row r="36" spans="2:22" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B36" s="27" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C36" s="27" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E36" s="27" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F36" s="27" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="G36" s="27" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="H36" s="29"/>
     </row>
     <row r="37" spans="2:22" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B37" s="31" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C37" s="27" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E37" s="27" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F37" s="27" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G37" s="27" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H37" s="29"/>
     </row>
     <row r="38" spans="2:22" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B38" s="31" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C38" s="27" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E38" s="27" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F38" s="27" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G38" s="27" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H38" s="29"/>
     </row>
     <row r="39" spans="2:22" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B39" s="31" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C39" s="27" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E39" s="27" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F39" s="27" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G39" s="27" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="H39" s="29"/>
     </row>
     <row r="40" spans="2:22" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B40" s="31" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C40" s="27" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E40" s="27" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F40" s="27" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="G40" s="27" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="H40" s="29"/>
     </row>
     <row r="41" spans="2:22" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B41" s="31" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C41" s="27" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E41" s="27" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F41" s="27" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="G41" s="27" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H41" s="29"/>
     </row>
     <row r="42" spans="2:22" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B42" s="31" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C42" s="27" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E42" s="27" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F42" s="27" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G42" s="27" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H42" s="29"/>
     </row>
     <row r="43" spans="2:22" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B43" s="31" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C43" s="27" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E43" s="27" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F43" s="27" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G43" s="27" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H43" s="29"/>
     </row>
     <row r="44" spans="2:22" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B44" s="31" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C44" s="27" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E44" s="27" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F44" s="27" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G44" s="27" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H44" s="29"/>
     </row>
     <row r="45" spans="2:22" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B45" s="31" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C45" s="27" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E45" s="27" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F45" s="27" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G45" s="27" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H45" s="29"/>
       <c r="M45" s="31"/>
@@ -3101,68 +3204,68 @@
     </row>
     <row r="46" spans="2:22" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B46" s="31" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C46" s="27" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F46" s="27" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G46" s="27" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="H46" s="29"/>
     </row>
     <row r="47" spans="2:22" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B47" s="31" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C47" s="27" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F47" s="27" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="G47" s="27" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H47" s="29"/>
     </row>
     <row r="48" spans="2:22" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B48" s="27" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C48" s="27" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E48" s="27" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F48" s="27" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G48" s="27" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H48" s="29"/>
       <c r="S48" s="32"/>
     </row>
     <row r="49" spans="2:22" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B49" s="27" t="s">
+        <v>113</v>
+      </c>
+      <c r="C49" s="27" t="s">
+        <v>130</v>
+      </c>
+      <c r="E49" s="27" t="s">
+        <v>190</v>
+      </c>
+      <c r="F49" s="27" t="s">
         <v>114</v>
       </c>
-      <c r="C49" s="27" t="s">
-        <v>131</v>
-      </c>
-      <c r="E49" s="27" t="s">
-        <v>191</v>
-      </c>
-      <c r="F49" s="27" t="s">
-        <v>115</v>
-      </c>
       <c r="G49" s="27" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H49" s="29"/>
       <c r="M49" s="31"/>
@@ -3178,19 +3281,19 @@
     </row>
     <row r="50" spans="2:22" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B50" s="27" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C50" s="27" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E50" s="27" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F50" s="27" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G50" s="27" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H50" s="29"/>
       <c r="M50" s="31"/>
@@ -3206,19 +3309,19 @@
     </row>
     <row r="51" spans="2:22" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B51" s="27" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C51" s="27" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E51" s="27" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F51" s="27" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G51" s="27" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H51" s="29"/>
       <c r="M51" s="31"/>
@@ -3234,19 +3337,19 @@
     </row>
     <row r="52" spans="2:22" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B52" s="31" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C52" s="27" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E52" s="34" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F52" s="31" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G52" s="27" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="H52" s="29"/>
       <c r="M52" s="31"/>
@@ -3262,19 +3365,19 @@
     </row>
     <row r="53" spans="2:22" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B53" s="31" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C53" s="27" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E53" s="34" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F53" s="31" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G53" s="27" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="H53" s="29"/>
       <c r="M53" s="31"/>
@@ -3292,19 +3395,19 @@
     </row>
     <row r="54" spans="2:22" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B54" s="31" t="s">
+        <v>105</v>
+      </c>
+      <c r="C54" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="E54" s="34" t="s">
         <v>106</v>
       </c>
-      <c r="C54" s="27" t="s">
-        <v>36</v>
-      </c>
-      <c r="E54" s="34" t="s">
+      <c r="F54" s="31" t="s">
         <v>107</v>
       </c>
-      <c r="F54" s="31" t="s">
-        <v>108</v>
-      </c>
       <c r="G54" s="27" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H54" s="29"/>
       <c r="M54" s="31"/>
@@ -3320,19 +3423,19 @@
     </row>
     <row r="55" spans="2:22" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B55" s="31" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C55" s="27" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E55" s="34" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F55" s="31" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="G55" s="27" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="H55" s="29"/>
       <c r="M55" s="31"/>
@@ -3348,19 +3451,19 @@
     </row>
     <row r="56" spans="2:22" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B56" s="31" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C56" s="31" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E56" s="34" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F56" s="31" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="G56" s="27" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H56" s="29"/>
       <c r="M56" s="31"/>
@@ -3376,19 +3479,19 @@
     </row>
     <row r="57" spans="2:22" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B57" s="31" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C57" s="31" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E57" s="34" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F57" s="31" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G57" s="27" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H57" s="29"/>
       <c r="M57" s="31"/>
@@ -3404,19 +3507,19 @@
     </row>
     <row r="58" spans="2:22" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B58" s="31" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C58" s="31" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E58" s="34" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F58" s="31" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="G58" s="27" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H58" s="29"/>
       <c r="M58" s="31"/>
@@ -3432,19 +3535,19 @@
     </row>
     <row r="59" spans="2:22" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B59" s="31" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C59" s="31" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E59" s="34" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F59" s="31" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="G59" s="27" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H59" s="29"/>
       <c r="M59" s="31"/>
@@ -3460,19 +3563,19 @@
     </row>
     <row r="60" spans="2:22" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B60" s="31" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C60" s="31" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E60" s="34" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F60" s="31" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="G60" s="27" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H60" s="29"/>
       <c r="M60" s="31"/>
@@ -3638,13 +3741,13 @@
         <v>25</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>31</v>
-      </c>
       <c r="F1" s="9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G1" s="6" t="s">
         <v>20</v>
@@ -3653,42 +3756,42 @@
         <v>2</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="J1" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="K1" s="8" t="s">
         <v>60</v>
-      </c>
-      <c r="K1" s="8" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:11" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="30" t="s">
+        <v>187</v>
+      </c>
+      <c r="C2" s="30" t="s">
         <v>188</v>
       </c>
-      <c r="C2" s="30" t="s">
-        <v>189</v>
-      </c>
       <c r="D2" s="27" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E2" s="30" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F2" s="34"/>
     </row>
     <row r="3" spans="1:11" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B3" s="28" t="s">
+        <v>187</v>
+      </c>
+      <c r="C3" s="28" t="s">
         <v>188</v>
       </c>
-      <c r="C3" s="28" t="s">
-        <v>189</v>
-      </c>
       <c r="D3" s="27" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E3" s="28" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F3" s="33"/>
     </row>
@@ -3716,14 +3819,14 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet6"/>
-  <dimension ref="A1:AA103"/>
+  <sheetPr codeName="Sheet6" filterMode="1"/>
+  <dimension ref="A1:AA161"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="80" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="L2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D7" sqref="D7"/>
+      <selection pane="bottomRight" activeCell="L163" sqref="L163"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3761,49 +3864,49 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="F1" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>96</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>97</v>
       </c>
       <c r="J1" s="7" t="s">
         <v>2</v>
       </c>
       <c r="K1" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="L1" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="M1" s="8" t="s">
         <v>26</v>
       </c>
       <c r="N1" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="O1" s="8" t="s">
         <v>27</v>
       </c>
       <c r="P1" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="Q1" s="4" t="s">
         <v>10</v>
@@ -3836,950 +3939,1450 @@
         <v>19</v>
       </c>
       <c r="AA1" s="7" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="2" spans="1:27" s="27" customFormat="1" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B2" s="27" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D2" s="27" t="s">
+        <v>78</v>
+      </c>
+      <c r="M2" s="31" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" s="27" t="s">
+        <v>119</v>
+      </c>
+      <c r="M3" s="31" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="27" t="s">
+        <v>204</v>
+      </c>
+      <c r="M4" s="31" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="27" t="s">
+        <v>120</v>
+      </c>
+      <c r="M5" s="27" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="27" t="s">
+        <v>205</v>
+      </c>
+      <c r="M6" s="31"/>
+    </row>
+    <row r="7" spans="1:27" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="27" t="s">
         <v>79</v>
       </c>
-      <c r="M2" s="31" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="3" spans="1:27" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="27" t="s">
-        <v>29</v>
-      </c>
-      <c r="D3" s="27" t="s">
+      <c r="M7" s="31" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="8" spans="1:27" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" s="27" t="s">
+        <v>206</v>
+      </c>
+      <c r="M8" s="31"/>
+    </row>
+    <row r="9" spans="1:27" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="27" t="s">
+        <v>207</v>
+      </c>
+      <c r="M9" s="31"/>
+    </row>
+    <row r="10" spans="1:27" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" s="27" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="11" spans="1:27" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="27" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="12" spans="1:27" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" s="27" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="13" spans="1:27" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" s="27" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="14" spans="1:27" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" s="27" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="15" spans="1:27" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="D15" s="27" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="16" spans="1:27" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="D16" s="27" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="17" spans="2:13" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="D17" s="27" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="18" spans="2:13" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="D18" s="27" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="19" spans="2:13" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="D19" s="27" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="20" spans="2:13" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="D20" s="27" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="21" spans="2:13" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="D21" s="31" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="22" spans="2:13" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="D22" s="27" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="23" spans="2:13" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="D23" s="27" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="24" spans="2:13" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="D24" s="27" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="25" spans="2:13" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="D25" s="27" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="26" spans="2:13" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="D26" s="27" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="27" spans="2:13" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="D27" s="27" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="28" spans="2:13" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="D28" s="27" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="29" spans="2:13" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="D29" s="27" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="30" spans="2:13" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="35" t="s">
+        <v>117</v>
+      </c>
+      <c r="D30" s="27" t="s">
+        <v>78</v>
+      </c>
+      <c r="M30" s="31" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="31" spans="2:13" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="35" t="s">
+        <v>117</v>
+      </c>
+      <c r="D31" s="27" t="s">
+        <v>119</v>
+      </c>
+      <c r="M31" s="31" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="32" spans="2:13" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="35" t="s">
+        <v>117</v>
+      </c>
+      <c r="D32" s="27" t="s">
+        <v>204</v>
+      </c>
+      <c r="M32" s="31" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="33" spans="2:13" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="35" t="s">
+        <v>117</v>
+      </c>
+      <c r="D33" s="27" t="s">
         <v>120</v>
       </c>
-      <c r="M3" s="31" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="4" spans="1:27" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="27" t="s">
-        <v>29</v>
-      </c>
-      <c r="D4" s="27" t="s">
+      <c r="M33" s="27" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="34" spans="2:13" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="35" t="s">
+        <v>117</v>
+      </c>
+      <c r="D34" s="27" t="s">
         <v>205</v>
       </c>
-      <c r="M4" s="31" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="5" spans="1:27" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="27" t="s">
-        <v>29</v>
-      </c>
-      <c r="D5" s="27" t="s">
+      <c r="M34" s="31"/>
+    </row>
+    <row r="35" spans="2:13" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B35" s="35" t="s">
+        <v>117</v>
+      </c>
+      <c r="D35" s="27" t="s">
+        <v>79</v>
+      </c>
+      <c r="M35" s="31" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="36" spans="2:13" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="35" t="s">
+        <v>117</v>
+      </c>
+      <c r="D36" s="27" t="s">
+        <v>206</v>
+      </c>
+      <c r="M36" s="31"/>
+    </row>
+    <row r="37" spans="2:13" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="35" t="s">
+        <v>117</v>
+      </c>
+      <c r="D37" s="27" t="s">
+        <v>207</v>
+      </c>
+      <c r="M37" s="31"/>
+    </row>
+    <row r="38" spans="2:13" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B38" s="35" t="s">
+        <v>117</v>
+      </c>
+      <c r="D38" s="27" t="s">
         <v>121</v>
       </c>
-      <c r="M5" s="27" t="s">
+    </row>
+    <row r="39" spans="2:13" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B39" s="35" t="s">
+        <v>117</v>
+      </c>
+      <c r="D39" s="31" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="40" spans="2:13" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B40" s="35" t="s">
+        <v>117</v>
+      </c>
+      <c r="D40" s="27" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="41" spans="2:13" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B41" s="35" t="s">
+        <v>117</v>
+      </c>
+      <c r="D41" s="27" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="42" spans="2:13" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B42" s="35" t="s">
+        <v>117</v>
+      </c>
+      <c r="D42" s="27" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="43" spans="2:13" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B43" s="35" t="s">
+        <v>117</v>
+      </c>
+      <c r="D43" s="27" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="44" spans="2:13" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B44" s="35" t="s">
+        <v>117</v>
+      </c>
+      <c r="D44" s="27" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="45" spans="2:13" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B45" s="35" t="s">
+        <v>117</v>
+      </c>
+      <c r="D45" s="27" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="46" spans="2:13" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B46" s="35" t="s">
+        <v>117</v>
+      </c>
+      <c r="D46" s="27" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="47" spans="2:13" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B47" s="35" t="s">
+        <v>117</v>
+      </c>
+      <c r="D47" s="27" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="48" spans="2:13" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B48" s="35" t="s">
+        <v>117</v>
+      </c>
+      <c r="D48" s="27" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="49" spans="2:13" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B49" s="35" t="s">
+        <v>117</v>
+      </c>
+      <c r="D49" s="31" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="50" spans="2:13" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B50" s="35" t="s">
+        <v>117</v>
+      </c>
+      <c r="D50" s="27" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="51" spans="2:13" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B51" s="35" t="s">
+        <v>117</v>
+      </c>
+      <c r="D51" s="27" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="52" spans="2:13" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B52" s="35" t="s">
+        <v>117</v>
+      </c>
+      <c r="D52" s="27" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="53" spans="2:13" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B53" s="31" t="s">
+        <v>199</v>
+      </c>
+      <c r="D53" s="27" t="s">
+        <v>119</v>
+      </c>
+      <c r="M53" s="31" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="54" spans="2:13" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B54" s="31" t="s">
+        <v>199</v>
+      </c>
+      <c r="D54" s="27" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="6" spans="1:27" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="27" t="s">
-        <v>29</v>
-      </c>
-      <c r="D6" s="27" t="s">
+      <c r="M54" s="31" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="55" spans="2:13" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B55" s="31" t="s">
+        <v>199</v>
+      </c>
+      <c r="D55" s="27" t="s">
+        <v>120</v>
+      </c>
+      <c r="M55" s="27" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="56" spans="2:13" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B56" s="31" t="s">
+        <v>199</v>
+      </c>
+      <c r="D56" s="27" t="s">
+        <v>205</v>
+      </c>
+      <c r="M56" s="31"/>
+    </row>
+    <row r="57" spans="2:13" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B57" s="31" t="s">
+        <v>199</v>
+      </c>
+      <c r="D57" s="27" t="s">
+        <v>79</v>
+      </c>
+      <c r="M57" s="31" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="58" spans="2:13" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B58" s="31" t="s">
+        <v>199</v>
+      </c>
+      <c r="D58" s="27" t="s">
         <v>206</v>
       </c>
-      <c r="M6" s="31"/>
-    </row>
-    <row r="7" spans="1:27" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="27" t="s">
-        <v>29</v>
-      </c>
-      <c r="D7" s="27" t="s">
-        <v>80</v>
-      </c>
-      <c r="M7" s="31" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="8" spans="1:27" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="27" t="s">
-        <v>29</v>
-      </c>
-      <c r="D8" s="27" t="s">
+      <c r="M58" s="31"/>
+    </row>
+    <row r="59" spans="2:13" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B59" s="31" t="s">
+        <v>199</v>
+      </c>
+      <c r="D59" s="27" t="s">
         <v>207</v>
       </c>
-      <c r="M8" s="31"/>
-    </row>
-    <row r="9" spans="1:27" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="27" t="s">
-        <v>29</v>
-      </c>
-      <c r="D9" s="27" t="s">
+      <c r="M59" s="31"/>
+    </row>
+    <row r="60" spans="2:13" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B60" s="31" t="s">
+        <v>199</v>
+      </c>
+      <c r="D60" s="27" t="s">
         <v>208</v>
       </c>
-      <c r="M9" s="31"/>
-    </row>
-    <row r="10" spans="1:27" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="27" t="s">
-        <v>29</v>
-      </c>
-      <c r="D10" s="27" t="s">
+    </row>
+    <row r="61" spans="2:13" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B61" s="31" t="s">
+        <v>199</v>
+      </c>
+      <c r="D61" s="31" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="11" spans="1:27" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="27" t="s">
-        <v>29</v>
-      </c>
-      <c r="D11" s="27" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="12" spans="1:27" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="27" t="s">
-        <v>29</v>
-      </c>
-      <c r="D12" s="27" t="s">
+    <row r="62" spans="2:13" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B62" s="31" t="s">
+        <v>199</v>
+      </c>
+      <c r="D62" s="27" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="63" spans="2:13" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B63" s="31" t="s">
+        <v>199</v>
+      </c>
+      <c r="D63" s="27" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="64" spans="2:13" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B64" s="31" t="s">
+        <v>199</v>
+      </c>
+      <c r="D64" s="27" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="65" spans="2:13" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B65" s="31" t="s">
+        <v>199</v>
+      </c>
+      <c r="D65" s="27" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="66" spans="2:13" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B66" s="31" t="s">
+        <v>199</v>
+      </c>
+      <c r="D66" s="27" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="67" spans="2:13" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B67" s="31" t="s">
+        <v>199</v>
+      </c>
+      <c r="D67" s="27" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="68" spans="2:13" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B68" s="31" t="s">
+        <v>199</v>
+      </c>
+      <c r="D68" s="27" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="69" spans="2:13" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B69" s="31" t="s">
+        <v>199</v>
+      </c>
+      <c r="D69" s="27" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="70" spans="2:13" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B70" s="31" t="s">
+        <v>199</v>
+      </c>
+      <c r="D70" s="27" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="71" spans="2:13" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B71" s="31" t="s">
+        <v>199</v>
+      </c>
+      <c r="D71" s="31" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="72" spans="2:13" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B72" s="31" t="s">
+        <v>199</v>
+      </c>
+      <c r="D72" s="27" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="73" spans="2:13" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B73" s="31" t="s">
+        <v>199</v>
+      </c>
+      <c r="D73" s="27" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="74" spans="2:13" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B74" s="31" t="s">
+        <v>199</v>
+      </c>
+      <c r="D74" s="27" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="75" spans="2:13" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B75" s="27" t="s">
+        <v>186</v>
+      </c>
+      <c r="D75" s="27" t="s">
+        <v>78</v>
+      </c>
+      <c r="M75" s="31" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="76" spans="2:13" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B76" s="27" t="s">
+        <v>186</v>
+      </c>
+      <c r="D76" s="27" t="s">
+        <v>119</v>
+      </c>
+      <c r="M76" s="31" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="77" spans="2:13" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B77" s="27" t="s">
+        <v>186</v>
+      </c>
+      <c r="D77" s="27" t="s">
+        <v>204</v>
+      </c>
+      <c r="M77" s="31" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="78" spans="2:13" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B78" s="27" t="s">
+        <v>186</v>
+      </c>
+      <c r="D78" s="27" t="s">
+        <v>120</v>
+      </c>
+      <c r="M78" s="27" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="79" spans="2:13" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B79" s="27" t="s">
+        <v>186</v>
+      </c>
+      <c r="D79" s="27" t="s">
+        <v>205</v>
+      </c>
+      <c r="M79" s="31"/>
+    </row>
+    <row r="80" spans="2:13" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B80" s="27" t="s">
+        <v>186</v>
+      </c>
+      <c r="D80" s="27" t="s">
+        <v>79</v>
+      </c>
+      <c r="M80" s="31" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="81" spans="2:13" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B81" s="27" t="s">
+        <v>186</v>
+      </c>
+      <c r="D81" s="27" t="s">
+        <v>206</v>
+      </c>
+      <c r="M81" s="31"/>
+    </row>
+    <row r="82" spans="2:13" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B82" s="27" t="s">
+        <v>186</v>
+      </c>
+      <c r="D82" s="27" t="s">
+        <v>207</v>
+      </c>
+      <c r="M82" s="31"/>
+    </row>
+    <row r="83" spans="2:13" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B83" s="27" t="s">
+        <v>186</v>
+      </c>
+      <c r="D83" s="27" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="84" spans="2:13" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B84" s="27" t="s">
+        <v>186</v>
+      </c>
+      <c r="D84" s="27" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="85" spans="2:13" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B85" s="27" t="s">
+        <v>186</v>
+      </c>
+      <c r="D85" s="27" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="86" spans="2:13" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B86" s="27" t="s">
+        <v>186</v>
+      </c>
+      <c r="D86" s="27" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="87" spans="2:13" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B87" s="27" t="s">
+        <v>186</v>
+      </c>
+      <c r="D87" s="27" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="88" spans="2:13" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B88" s="27" t="s">
+        <v>186</v>
+      </c>
+      <c r="D88" s="27" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="89" spans="2:13" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B89" s="27" t="s">
+        <v>186</v>
+      </c>
+      <c r="D89" s="27" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="90" spans="2:13" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B90" s="27" t="s">
+        <v>186</v>
+      </c>
+      <c r="D90" s="27" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="91" spans="2:13" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B91" s="27" t="s">
+        <v>186</v>
+      </c>
+      <c r="D91" s="31" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="92" spans="2:13" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B92" s="27" t="s">
+        <v>186</v>
+      </c>
+      <c r="D92" s="27" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="93" spans="2:13" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B93" s="27" t="s">
+        <v>186</v>
+      </c>
+      <c r="D93" s="27" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="94" spans="2:13" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B94" s="35" t="s">
+        <v>186</v>
+      </c>
+      <c r="D94" s="27" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="95" spans="2:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B95" s="35" t="s">
+        <v>186</v>
+      </c>
+      <c r="C95" s="27" t="s">
+        <v>188</v>
+      </c>
+      <c r="D95" s="31" t="s">
+        <v>191</v>
+      </c>
+      <c r="E95" s="27" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="96" spans="2:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B96" s="35" t="s">
+        <v>186</v>
+      </c>
+      <c r="C96" s="27" t="s">
+        <v>188</v>
+      </c>
+      <c r="D96" s="31" t="s">
+        <v>240</v>
+      </c>
+      <c r="E96" s="27" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="97" spans="2:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B97" s="35" t="s">
+        <v>186</v>
+      </c>
+      <c r="C97" s="27" t="s">
+        <v>188</v>
+      </c>
+      <c r="D97" s="31" t="s">
+        <v>105</v>
+      </c>
+      <c r="E97" s="27" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="98" spans="2:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B98" s="35" t="s">
+        <v>186</v>
+      </c>
+      <c r="C98" s="27" t="s">
+        <v>188</v>
+      </c>
+      <c r="D98" s="31" t="s">
+        <v>192</v>
+      </c>
+      <c r="E98" s="27" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="99" spans="2:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B99" s="35" t="s">
+        <v>186</v>
+      </c>
+      <c r="C99" s="27" t="s">
+        <v>188</v>
+      </c>
+      <c r="D99" s="31" t="s">
+        <v>207</v>
+      </c>
+      <c r="E99" s="27" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="100" spans="2:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B100" s="35" t="s">
+        <v>186</v>
+      </c>
+      <c r="C100" s="27" t="s">
+        <v>188</v>
+      </c>
+      <c r="D100" s="31" t="s">
+        <v>241</v>
+      </c>
+      <c r="E100" s="27" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="101" spans="2:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B101" s="35" t="s">
+        <v>186</v>
+      </c>
+      <c r="C101" s="27" t="s">
+        <v>188</v>
+      </c>
+      <c r="D101" s="31" t="s">
+        <v>242</v>
+      </c>
+      <c r="E101" s="27" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="102" spans="2:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B102" s="35" t="s">
+        <v>186</v>
+      </c>
+      <c r="C102" s="27" t="s">
+        <v>188</v>
+      </c>
+      <c r="D102" s="31" t="s">
+        <v>243</v>
+      </c>
+      <c r="E102" s="27" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="103" spans="2:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B103" s="35" t="s">
+        <v>186</v>
+      </c>
+      <c r="C103" s="27" t="s">
+        <v>188</v>
+      </c>
+      <c r="D103" s="31" t="s">
+        <v>244</v>
+      </c>
+      <c r="E103" s="27" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="104" spans="2:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B104" s="35" t="s">
+        <v>247</v>
+      </c>
+      <c r="D104" s="27" t="s">
+        <v>78</v>
+      </c>
+      <c r="M104" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="105" spans="2:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B105" s="35" t="s">
+        <v>247</v>
+      </c>
+      <c r="D105" s="27" t="s">
+        <v>119</v>
+      </c>
+      <c r="M105" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="106" spans="2:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B106" s="35" t="s">
+        <v>247</v>
+      </c>
+      <c r="D106" s="27" t="s">
+        <v>253</v>
+      </c>
+      <c r="M106" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="107" spans="2:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B107" s="35" t="s">
+        <v>247</v>
+      </c>
+      <c r="D107" s="27" t="s">
+        <v>120</v>
+      </c>
+      <c r="M107" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="108" spans="2:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B108" s="35" t="s">
+        <v>247</v>
+      </c>
+      <c r="D108" s="27" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="109" spans="2:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B109" s="35" t="s">
+        <v>247</v>
+      </c>
+      <c r="D109" s="27" t="s">
+        <v>79</v>
+      </c>
+      <c r="M109" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="110" spans="2:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B110" s="35" t="s">
+        <v>247</v>
+      </c>
+      <c r="D110" s="27" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="111" spans="2:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B111" s="35" t="s">
+        <v>247</v>
+      </c>
+      <c r="D111" s="27" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="112" spans="2:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B112" s="35" t="s">
+        <v>247</v>
+      </c>
+      <c r="D112" s="27" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="113" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B113" s="35" t="s">
+        <v>247</v>
+      </c>
+      <c r="D113" s="31" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="114" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B114" s="35" t="s">
+        <v>247</v>
+      </c>
+      <c r="D114" s="27" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="115" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B115" s="35" t="s">
+        <v>247</v>
+      </c>
+      <c r="D115" s="27" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="116" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B116" s="35" t="s">
+        <v>247</v>
+      </c>
+      <c r="D116" s="27" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="117" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B117" s="35" t="s">
+        <v>247</v>
+      </c>
+      <c r="D117" s="27" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="118" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B118" s="35" t="s">
+        <v>247</v>
+      </c>
+      <c r="D118" s="27" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="119" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B119" s="35" t="s">
+        <v>247</v>
+      </c>
+      <c r="D119" s="27" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="120" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B120" s="35" t="s">
+        <v>247</v>
+      </c>
+      <c r="D120" s="27" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="121" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B121" s="35" t="s">
+        <v>247</v>
+      </c>
+      <c r="D121" s="27" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="122" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B122" s="35" t="s">
+        <v>247</v>
+      </c>
+      <c r="D122" s="27" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="123" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B123" s="35" t="s">
+        <v>247</v>
+      </c>
+      <c r="D123" s="31" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="124" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B124" s="35" t="s">
+        <v>247</v>
+      </c>
+      <c r="D124" s="27" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="125" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B125" s="35" t="s">
+        <v>247</v>
+      </c>
+      <c r="D125" s="27" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="126" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B126" s="35" t="s">
+        <v>247</v>
+      </c>
+      <c r="D126" s="27" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="127" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B127" s="31" t="s">
+        <v>247</v>
+      </c>
+      <c r="D127" s="27" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="128" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B128" s="31" t="s">
+        <v>247</v>
+      </c>
+      <c r="D128" s="27" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="129" spans="2:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B129" s="35" t="s">
+        <v>247</v>
+      </c>
+      <c r="D129" s="27" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="130" spans="2:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B130" s="35" t="s">
+        <v>247</v>
+      </c>
+      <c r="D130" s="27" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="13" spans="1:27" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="27" t="s">
-        <v>29</v>
-      </c>
-      <c r="D13" s="27" t="s">
+    <row r="131" spans="2:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B131" s="35" t="s">
+        <v>247</v>
+      </c>
+      <c r="D131" s="27" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="132" spans="2:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B132" s="27" t="s">
+        <v>121</v>
+      </c>
+      <c r="D132" s="27" t="s">
+        <v>119</v>
+      </c>
+      <c r="M132" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="133" spans="2:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B133" s="27" t="s">
+        <v>121</v>
+      </c>
+      <c r="D133" s="27" t="s">
+        <v>253</v>
+      </c>
+      <c r="M133" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="134" spans="2:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B134" s="27" t="s">
+        <v>121</v>
+      </c>
+      <c r="D134" s="27" t="s">
+        <v>120</v>
+      </c>
+      <c r="M134" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="135" spans="2:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B135" s="27" t="s">
+        <v>121</v>
+      </c>
+      <c r="D135" s="27" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="136" spans="2:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B136" s="27" t="s">
+        <v>121</v>
+      </c>
+      <c r="D136" s="27" t="s">
+        <v>79</v>
+      </c>
+      <c r="M136" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="137" spans="2:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B137" s="27" t="s">
+        <v>121</v>
+      </c>
+      <c r="D137" s="27" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="138" spans="2:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B138" s="27" t="s">
+        <v>121</v>
+      </c>
+      <c r="D138" s="27" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="139" spans="2:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B139" s="27" t="s">
+        <v>121</v>
+      </c>
+      <c r="D139" s="27" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="140" spans="2:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B140" s="27" t="s">
+        <v>121</v>
+      </c>
+      <c r="D140" s="31" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="141" spans="2:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B141" s="27" t="s">
+        <v>121</v>
+      </c>
+      <c r="D141" s="27" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="142" spans="2:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B142" s="27" t="s">
+        <v>121</v>
+      </c>
+      <c r="D142" s="27" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="143" spans="2:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B143" s="27" t="s">
+        <v>121</v>
+      </c>
+      <c r="D143" s="27" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="144" spans="2:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B144" s="27" t="s">
+        <v>121</v>
+      </c>
+      <c r="D144" s="27" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="145" spans="2:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B145" s="27" t="s">
+        <v>121</v>
+      </c>
+      <c r="D145" s="27" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="146" spans="2:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B146" s="27" t="s">
+        <v>121</v>
+      </c>
+      <c r="D146" s="27" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="147" spans="2:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B147" s="27" t="s">
+        <v>121</v>
+      </c>
+      <c r="D147" s="27" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="148" spans="2:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B148" s="27" t="s">
+        <v>121</v>
+      </c>
+      <c r="D148" s="27" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="149" spans="2:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B149" s="27" t="s">
+        <v>121</v>
+      </c>
+      <c r="D149" s="27" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="150" spans="2:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B150" s="27" t="s">
+        <v>121</v>
+      </c>
+      <c r="D150" s="31" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="151" spans="2:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B151" s="27" t="s">
+        <v>121</v>
+      </c>
+      <c r="D151" s="27" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="152" spans="2:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B152" s="27" t="s">
+        <v>121</v>
+      </c>
+      <c r="D152" s="27" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="14" spans="1:27" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="27" t="s">
-        <v>29</v>
-      </c>
-      <c r="D14" s="27" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="15" spans="1:27" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="27" t="s">
-        <v>29</v>
-      </c>
-      <c r="D15" s="27" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="16" spans="1:27" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="27" t="s">
-        <v>29</v>
-      </c>
-      <c r="D16" s="27" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="17" spans="2:13" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="27" t="s">
-        <v>29</v>
-      </c>
-      <c r="D17" s="27" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="18" spans="2:13" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="27" t="s">
-        <v>29</v>
-      </c>
-      <c r="D18" s="27" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="19" spans="2:13" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="27" t="s">
-        <v>29</v>
-      </c>
-      <c r="D19" s="27" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="20" spans="2:13" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="27" t="s">
-        <v>29</v>
-      </c>
-      <c r="D20" s="27" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="21" spans="2:13" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="27" t="s">
-        <v>29</v>
-      </c>
-      <c r="D21" s="31" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="22" spans="2:13" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="27" t="s">
-        <v>29</v>
-      </c>
-      <c r="D22" s="27" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="23" spans="2:13" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="27" t="s">
-        <v>29</v>
-      </c>
-      <c r="D23" s="27" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="24" spans="2:13" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="35" t="s">
-        <v>29</v>
-      </c>
-      <c r="D24" s="27" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="25" spans="2:13" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="27" t="s">
-        <v>29</v>
-      </c>
-      <c r="D25" s="27" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="26" spans="2:13" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="27" t="s">
-        <v>29</v>
-      </c>
-      <c r="D26" s="27" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="27" spans="2:13" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="35" t="s">
-        <v>29</v>
-      </c>
-      <c r="D27" s="27" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="28" spans="2:13" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="35" t="s">
-        <v>29</v>
-      </c>
-      <c r="D28" s="27" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="29" spans="2:13" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="35" t="s">
-        <v>29</v>
-      </c>
-      <c r="D29" s="27" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="30" spans="2:13" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="35" t="s">
-        <v>118</v>
-      </c>
-      <c r="D30" s="27" t="s">
+    <row r="153" spans="2:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B153" s="35" t="s">
+        <v>121</v>
+      </c>
+      <c r="D153" s="27" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="154" spans="2:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B154" s="27" t="s">
+        <v>121</v>
+      </c>
+      <c r="D154" s="27" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="155" spans="2:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B155" s="27" t="s">
+        <v>121</v>
+      </c>
+      <c r="D155" s="27" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="156" spans="2:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B156" s="35" t="s">
+        <v>121</v>
+      </c>
+      <c r="D156" s="27" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="157" spans="2:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B157" s="35" t="s">
+        <v>121</v>
+      </c>
+      <c r="D157" s="27" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="158" spans="2:13" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B158" s="35" t="s">
+        <v>121</v>
+      </c>
+      <c r="D158" s="27" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="159" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B159" s="27" t="s">
+        <v>270</v>
+      </c>
+      <c r="D159" s="27" t="s">
         <v>79</v>
       </c>
-      <c r="M30" s="31" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="31" spans="2:13" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="35" t="s">
-        <v>118</v>
-      </c>
-      <c r="D31" s="27" t="s">
-        <v>120</v>
-      </c>
-      <c r="M31" s="31" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="32" spans="2:13" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="35" t="s">
-        <v>118</v>
-      </c>
-      <c r="D32" s="27" t="s">
-        <v>205</v>
-      </c>
-      <c r="M32" s="31" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="33" spans="2:13" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="35" t="s">
-        <v>118</v>
-      </c>
-      <c r="D33" s="27" t="s">
-        <v>121</v>
-      </c>
-      <c r="M33" s="27" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="34" spans="2:13" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="35" t="s">
-        <v>118</v>
-      </c>
-      <c r="D34" s="27" t="s">
-        <v>206</v>
-      </c>
-      <c r="M34" s="31"/>
-    </row>
-    <row r="35" spans="2:13" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="35" t="s">
-        <v>118</v>
-      </c>
-      <c r="D35" s="27" t="s">
-        <v>80</v>
-      </c>
-      <c r="M35" s="31" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="36" spans="2:13" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="35" t="s">
-        <v>118</v>
-      </c>
-      <c r="D36" s="27" t="s">
-        <v>207</v>
-      </c>
-      <c r="M36" s="31"/>
-    </row>
-    <row r="37" spans="2:13" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="35" t="s">
-        <v>118</v>
-      </c>
-      <c r="D37" s="27" t="s">
-        <v>208</v>
-      </c>
-      <c r="M37" s="31"/>
-    </row>
-    <row r="38" spans="2:13" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="35" t="s">
-        <v>118</v>
-      </c>
-      <c r="D38" s="27" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="39" spans="2:13" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="35" t="s">
-        <v>118</v>
-      </c>
-      <c r="D39" s="31" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="40" spans="2:13" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="35" t="s">
-        <v>118</v>
-      </c>
-      <c r="D40" s="27" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="41" spans="2:13" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="35" t="s">
-        <v>118</v>
-      </c>
-      <c r="D41" s="27" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="42" spans="2:13" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="35" t="s">
-        <v>118</v>
-      </c>
-      <c r="D42" s="27" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="43" spans="2:13" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="35" t="s">
-        <v>118</v>
-      </c>
-      <c r="D43" s="27" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="44" spans="2:13" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="35" t="s">
-        <v>118</v>
-      </c>
-      <c r="D44" s="27" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="45" spans="2:13" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="35" t="s">
-        <v>118</v>
-      </c>
-      <c r="D45" s="27" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="46" spans="2:13" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="35" t="s">
-        <v>118</v>
-      </c>
-      <c r="D46" s="27" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="47" spans="2:13" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="35" t="s">
-        <v>118</v>
-      </c>
-      <c r="D47" s="27" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="48" spans="2:13" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="35" t="s">
-        <v>118</v>
-      </c>
-      <c r="D48" s="27" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="49" spans="2:13" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B49" s="35" t="s">
-        <v>118</v>
-      </c>
-      <c r="D49" s="31" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="50" spans="2:13" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="35" t="s">
-        <v>118</v>
-      </c>
-      <c r="D50" s="27" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="51" spans="2:13" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B51" s="35" t="s">
-        <v>118</v>
-      </c>
-      <c r="D51" s="27" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="52" spans="2:13" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="35" t="s">
-        <v>118</v>
-      </c>
-      <c r="D52" s="27" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="53" spans="2:13" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B53" s="31" t="s">
-        <v>200</v>
-      </c>
-      <c r="D53" s="27" t="s">
-        <v>120</v>
-      </c>
-      <c r="M53" s="31" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="54" spans="2:13" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B54" s="31" t="s">
-        <v>200</v>
-      </c>
-      <c r="D54" s="27" t="s">
-        <v>205</v>
-      </c>
-      <c r="M54" s="31" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="55" spans="2:13" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B55" s="31" t="s">
-        <v>200</v>
-      </c>
-      <c r="D55" s="27" t="s">
-        <v>121</v>
-      </c>
-      <c r="M55" s="27" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="56" spans="2:13" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B56" s="31" t="s">
-        <v>200</v>
-      </c>
-      <c r="D56" s="27" t="s">
-        <v>206</v>
-      </c>
-      <c r="M56" s="31"/>
-    </row>
-    <row r="57" spans="2:13" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B57" s="31" t="s">
-        <v>200</v>
-      </c>
-      <c r="D57" s="27" t="s">
-        <v>80</v>
-      </c>
-      <c r="M57" s="31" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="58" spans="2:13" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B58" s="31" t="s">
-        <v>200</v>
-      </c>
-      <c r="D58" s="27" t="s">
-        <v>207</v>
-      </c>
-      <c r="M58" s="31"/>
-    </row>
-    <row r="59" spans="2:13" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B59" s="31" t="s">
-        <v>200</v>
-      </c>
-      <c r="D59" s="27" t="s">
-        <v>208</v>
-      </c>
-      <c r="M59" s="31"/>
-    </row>
-    <row r="60" spans="2:13" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B60" s="31" t="s">
-        <v>200</v>
-      </c>
-      <c r="D60" s="27" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="61" spans="2:13" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B61" s="31" t="s">
-        <v>200</v>
-      </c>
-      <c r="D61" s="31" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="62" spans="2:13" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B62" s="31" t="s">
-        <v>200</v>
-      </c>
-      <c r="D62" s="27" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="63" spans="2:13" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B63" s="31" t="s">
-        <v>200</v>
-      </c>
-      <c r="D63" s="27" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="64" spans="2:13" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B64" s="31" t="s">
-        <v>200</v>
-      </c>
-      <c r="D64" s="27" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="65" spans="2:13" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B65" s="31" t="s">
-        <v>200</v>
-      </c>
-      <c r="D65" s="27" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="66" spans="2:13" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B66" s="31" t="s">
-        <v>200</v>
-      </c>
-      <c r="D66" s="27" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="67" spans="2:13" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B67" s="31" t="s">
-        <v>200</v>
-      </c>
-      <c r="D67" s="27" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="68" spans="2:13" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B68" s="31" t="s">
-        <v>200</v>
-      </c>
-      <c r="D68" s="27" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="69" spans="2:13" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B69" s="31" t="s">
-        <v>200</v>
-      </c>
-      <c r="D69" s="27" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="70" spans="2:13" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B70" s="31" t="s">
-        <v>200</v>
-      </c>
-      <c r="D70" s="27" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="71" spans="2:13" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B71" s="31" t="s">
-        <v>200</v>
-      </c>
-      <c r="D71" s="31" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="72" spans="2:13" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B72" s="31" t="s">
-        <v>200</v>
-      </c>
-      <c r="D72" s="27" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="73" spans="2:13" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B73" s="31" t="s">
-        <v>200</v>
-      </c>
-      <c r="D73" s="27" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="74" spans="2:13" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B74" s="31" t="s">
-        <v>200</v>
-      </c>
-      <c r="D74" s="27" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="75" spans="2:13" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B75" s="27" t="s">
-        <v>187</v>
-      </c>
-      <c r="D75" s="27" t="s">
-        <v>79</v>
-      </c>
-      <c r="M75" s="31" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="76" spans="2:13" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B76" s="27" t="s">
-        <v>187</v>
-      </c>
-      <c r="D76" s="27" t="s">
-        <v>120</v>
-      </c>
-      <c r="M76" s="31" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="77" spans="2:13" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B77" s="27" t="s">
-        <v>187</v>
-      </c>
-      <c r="D77" s="27" t="s">
-        <v>205</v>
-      </c>
-      <c r="M77" s="31" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="78" spans="2:13" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B78" s="27" t="s">
-        <v>187</v>
-      </c>
-      <c r="D78" s="27" t="s">
-        <v>121</v>
-      </c>
-      <c r="M78" s="27" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="79" spans="2:13" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B79" s="27" t="s">
-        <v>187</v>
-      </c>
-      <c r="D79" s="27" t="s">
-        <v>206</v>
-      </c>
-      <c r="M79" s="31"/>
-    </row>
-    <row r="80" spans="2:13" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B80" s="27" t="s">
-        <v>187</v>
-      </c>
-      <c r="D80" s="27" t="s">
-        <v>80</v>
-      </c>
-      <c r="M80" s="31" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="81" spans="2:13" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B81" s="27" t="s">
-        <v>187</v>
-      </c>
-      <c r="D81" s="27" t="s">
-        <v>207</v>
-      </c>
-      <c r="M81" s="31"/>
-    </row>
-    <row r="82" spans="2:13" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B82" s="27" t="s">
-        <v>187</v>
-      </c>
-      <c r="D82" s="27" t="s">
-        <v>208</v>
-      </c>
-      <c r="M82" s="31"/>
-    </row>
-    <row r="83" spans="2:13" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B83" s="27" t="s">
-        <v>187</v>
-      </c>
-      <c r="D83" s="27" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="84" spans="2:13" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B84" s="27" t="s">
-        <v>187</v>
-      </c>
-      <c r="D84" s="27" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="85" spans="2:13" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B85" s="27" t="s">
-        <v>187</v>
-      </c>
-      <c r="D85" s="27" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="86" spans="2:13" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B86" s="27" t="s">
-        <v>187</v>
-      </c>
-      <c r="D86" s="27" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="87" spans="2:13" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B87" s="27" t="s">
-        <v>187</v>
-      </c>
-      <c r="D87" s="27" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="88" spans="2:13" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B88" s="27" t="s">
-        <v>187</v>
-      </c>
-      <c r="D88" s="27" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="89" spans="2:13" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B89" s="27" t="s">
-        <v>187</v>
-      </c>
-      <c r="D89" s="27" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="90" spans="2:13" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B90" s="27" t="s">
-        <v>187</v>
-      </c>
-      <c r="D90" s="27" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="91" spans="2:13" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B91" s="27" t="s">
-        <v>187</v>
-      </c>
-      <c r="D91" s="31" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="92" spans="2:13" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B92" s="27" t="s">
-        <v>187</v>
-      </c>
-      <c r="D92" s="27" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="93" spans="2:13" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B93" s="27" t="s">
-        <v>187</v>
-      </c>
-      <c r="D93" s="27" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="94" spans="2:13" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B94" s="35" t="s">
-        <v>187</v>
-      </c>
-      <c r="D94" s="27" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="95" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B95" s="35" t="s">
-        <v>187</v>
-      </c>
-      <c r="C95" s="27" t="s">
-        <v>189</v>
-      </c>
-      <c r="D95" s="31" t="s">
-        <v>192</v>
-      </c>
-      <c r="E95" s="27" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="96" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B96" s="35" t="s">
-        <v>187</v>
-      </c>
-      <c r="C96" s="27" t="s">
-        <v>189</v>
-      </c>
-      <c r="D96" s="31" t="s">
-        <v>241</v>
-      </c>
-      <c r="E96" s="27" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="97" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B97" s="35" t="s">
-        <v>187</v>
-      </c>
-      <c r="C97" s="27" t="s">
-        <v>189</v>
-      </c>
-      <c r="D97" s="31" t="s">
-        <v>106</v>
-      </c>
-      <c r="E97" s="27" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="98" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B98" s="35" t="s">
-        <v>187</v>
-      </c>
-      <c r="C98" s="27" t="s">
-        <v>189</v>
-      </c>
-      <c r="D98" s="31" t="s">
-        <v>193</v>
-      </c>
-      <c r="E98" s="27" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="99" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B99" s="35" t="s">
-        <v>187</v>
-      </c>
-      <c r="C99" s="27" t="s">
-        <v>189</v>
-      </c>
-      <c r="D99" s="31" t="s">
-        <v>208</v>
-      </c>
-      <c r="E99" s="27" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="100" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B100" s="35" t="s">
-        <v>187</v>
-      </c>
-      <c r="C100" s="27" t="s">
-        <v>189</v>
-      </c>
-      <c r="D100" s="31" t="s">
-        <v>242</v>
-      </c>
-      <c r="E100" s="27" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="101" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B101" s="35" t="s">
-        <v>187</v>
-      </c>
-      <c r="C101" s="27" t="s">
-        <v>189</v>
-      </c>
-      <c r="D101" s="31" t="s">
-        <v>243</v>
-      </c>
-      <c r="E101" s="27" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="102" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B102" s="35" t="s">
-        <v>187</v>
-      </c>
-      <c r="C102" s="27" t="s">
-        <v>189</v>
-      </c>
-      <c r="D102" s="31" t="s">
-        <v>244</v>
-      </c>
-      <c r="E102" s="27" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="103" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B103" s="35" t="s">
-        <v>187</v>
-      </c>
-      <c r="C103" s="27" t="s">
-        <v>189</v>
-      </c>
-      <c r="D103" s="31" t="s">
-        <v>245</v>
-      </c>
-      <c r="E103" s="27" t="s">
-        <v>189</v>
+      <c r="M159" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="160" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B160" s="27" t="s">
+        <v>270</v>
+      </c>
+      <c r="D160" s="27" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="161" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B161" s="27" t="s">
+        <v>270</v>
+      </c>
+      <c r="D161" s="27" t="s">
+        <v>263</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AA9"/>
+  <autoFilter ref="A1:AA161">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="category"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <customSheetViews>
     <customSheetView guid="{BF8E1B46-AD75-6E4F-85B7-6E6C75F2AAA2}" scale="130" filter="1" showAutoFilter="1" hiddenRows="1">
       <selection activeCell="E10" sqref="E10"/>
@@ -4831,16 +5434,16 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>2</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -4897,28 +5500,28 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>71</v>
-      </c>
       <c r="E1" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H1" s="8" t="s">
         <v>26</v>
       </c>
       <c r="I1" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J1" s="8" t="s">
         <v>27</v>
@@ -4927,7 +5530,7 @@
         <v>2</v>
       </c>
       <c r="L1" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -4975,28 +5578,28 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>91</v>
-      </c>
       <c r="H1" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="I1" s="8" t="s">
         <v>60</v>
-      </c>
-      <c r="I1" s="8" t="s">
-        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>